<commit_message>
Modification on the whole library
</commit_message>
<xml_diff>
--- a/计科1703面向对象分组统计表.xlsx
+++ b/计科1703面向对象分组统计表.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Codes\cpp-Object-oriented-Programming\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC72DFBB-0760-4601-A6AF-6DB296C1A62A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0AFAF53-848C-43A5-B438-98F9FB4C4D94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -543,7 +543,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -579,7 +579,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3">
-        <v>1</v>
+        <v>170301</v>
       </c>
       <c r="B3" t="s">
         <v>18</v>
@@ -604,7 +604,7 @@
     </row>
     <row r="5" spans="1:5" ht="15.75">
       <c r="A5">
-        <v>2</v>
+        <v>170302</v>
       </c>
       <c r="B5" t="s">
         <v>28</v>
@@ -629,7 +629,7 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7">
-        <v>3</v>
+        <v>170303</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
@@ -665,7 +665,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10">
-        <v>4</v>
+        <v>170304</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
@@ -690,7 +690,7 @@
     </row>
     <row r="13" spans="1:5">
       <c r="A13">
-        <v>5</v>
+        <v>170305</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>40</v>
@@ -704,7 +704,7 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14">
-        <v>6</v>
+        <v>170306</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>25</v>
@@ -718,7 +718,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15">
-        <v>7</v>
+        <v>170307</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>41</v>
@@ -732,7 +732,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16">
-        <v>8</v>
+        <v>170308</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>37</v>
@@ -746,7 +746,7 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17">
-        <v>9</v>
+        <v>170309</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>23</v>
@@ -760,7 +760,7 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18">
-        <v>10</v>
+        <v>170310</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>39</v>
@@ -774,7 +774,7 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19">
-        <v>11</v>
+        <v>170311</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>22</v>
@@ -788,7 +788,7 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20">
-        <v>12</v>
+        <v>170312</v>
       </c>
       <c r="B20" t="s">
         <v>16</v>
@@ -802,7 +802,7 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21">
-        <v>13</v>
+        <v>170313</v>
       </c>
       <c r="B21" t="s">
         <v>14</v>
@@ -816,7 +816,7 @@
     </row>
     <row r="22" spans="1:4">
       <c r="A22">
-        <v>14</v>
+        <v>170314</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>32</v>
@@ -830,7 +830,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23">
-        <v>15</v>
+        <v>170315</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>24</v>
@@ -844,7 +844,7 @@
     </row>
     <row r="24" spans="1:4">
       <c r="A24">
-        <v>16</v>
+        <v>170316</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>38</v>
@@ -858,7 +858,7 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25">
-        <v>17</v>
+        <v>170317</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>26</v>
@@ -872,7 +872,7 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26">
-        <v>18</v>
+        <v>170318</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>27</v>
@@ -886,7 +886,7 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27">
-        <v>19</v>
+        <v>170319</v>
       </c>
       <c r="B27" t="s">
         <v>13</v>
@@ -900,7 +900,7 @@
     </row>
     <row r="28" spans="1:4">
       <c r="A28">
-        <v>20</v>
+        <v>170320</v>
       </c>
       <c r="B28" t="s">
         <v>12</v>
@@ -914,7 +914,7 @@
     </row>
     <row r="29" spans="1:4">
       <c r="A29">
-        <v>21</v>
+        <v>170321</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>36</v>

</xml_diff>